<commit_message>
Auto stash before merge of "master" and "gitee/master"
</commit_message>
<xml_diff>
--- a/res/constraints.xlsx
+++ b/res/constraints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LaserController\LaserController\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8838A516-D595-448F-9A90-7B34F539B7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C39DFB1-E4D8-4AF2-B035-322025D46514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5385" yWindow="-21720" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1571,7 +1571,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomRight" activeCell="T17" sqref="T17:AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>